<commit_message>
complete ShopController and normal Controller
</commit_message>
<xml_diff>
--- a/public/data-excel.xlsx
+++ b/public/data-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0-A-0\Projects\php\noir-laravel-shop-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CF1238-6BBE-426F-A272-B6CF44D17BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE8A9D7-5298-48DD-9411-AD10EB71B321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7845" yWindow="45" windowWidth="21075" windowHeight="11385" xr2:uid="{FD199194-9733-4EA9-A27F-0A4F6154EB81}"/>
+    <workbookView xWindow="7725" yWindow="45" windowWidth="21075" windowHeight="11385" xr2:uid="{FD199194-9733-4EA9-A27F-0A4F6154EB81}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -891,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3040E10-72E2-4B29-8B2A-19F11F15320E}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,233 +946,233 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="195" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>227</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>199</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>140</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>257</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>287</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>355</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>355</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>257</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="195" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>287</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>457</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>297</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>595</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>597</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>499</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>697</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>387</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>427</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>557</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>557</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>425</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>497</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="3" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>